<commit_message>
added file selection dialog
</commit_message>
<xml_diff>
--- a/test/testData.xlsx
+++ b/test/testData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guusd\Documents\GitHub\dataverwerking\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\554766\Documents\Dataverwerking\dataverwerking\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6A1D3A4-CB01-4172-ACC4-B65A18098AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF8DDC2-4FF7-42C1-86D7-897698F40FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
   </bookViews>
   <sheets>
-    <sheet name="|Toets 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="3" r:id="rId1"/>
+    <sheet name="|Toets 1" sheetId="1" r:id="rId2"/>
+    <sheet name="|Toets 2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>Naam toets</t>
   </si>
@@ -51,6 +53,99 @@
   </si>
   <si>
     <t>N-term:</t>
+  </si>
+  <si>
+    <t>Voornaam</t>
+  </si>
+  <si>
+    <t>achternaam</t>
+  </si>
+  <si>
+    <t>klas</t>
+  </si>
+  <si>
+    <t>Vraag 1</t>
+  </si>
+  <si>
+    <t>Moeilijkheidsgraad</t>
+  </si>
+  <si>
+    <t>Type vraag</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Vraag 2</t>
+  </si>
+  <si>
+    <t>Vraag 3</t>
+  </si>
+  <si>
+    <t>Vraag 4</t>
+  </si>
+  <si>
+    <t>Vraag 5</t>
+  </si>
+  <si>
+    <t>Vraag 6</t>
+  </si>
+  <si>
+    <t>Max aantal punten</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Klaassen</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>de Beer</t>
+  </si>
+  <si>
+    <t>G1A</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>de Boer</t>
+  </si>
+  <si>
+    <t>G1B</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>MF</t>
   </si>
 </sst>
 </file>
@@ -94,7 +189,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,20 +520,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F662D5-C154-478B-901C-CD18525D5839}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE63FB54-0172-4D28-B685-FF98F11F42E1}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F662D5-C154-478B-901C-CD18525D5839}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -465,6 +621,441 @@
         <v>4</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF6D0A-3344-44E1-B4F6-C7514DC4A2F0}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44986</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished up data import
</commit_message>
<xml_diff>
--- a/test/testData.xlsx
+++ b/test/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\554766\Documents\Dataverwerking\dataverwerking\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guusd\Documents\GitHub\dataverwerking\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF8DDC2-4FF7-42C1-86D7-897698F40FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF2652B-B2F7-4623-872A-4EA28D94CE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Naam toets</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>MF</t>
+  </si>
+  <si>
+    <t>aantal vragen:</t>
+  </si>
+  <si>
+    <t>Aantal vragen:</t>
   </si>
 </sst>
 </file>
@@ -189,7 +195,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -205,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,13 +529,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE63FB54-0172-4D28-B685-FF98F11F42E1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -537,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -545,7 +551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -553,7 +559,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -561,7 +567,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -569,7 +575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -583,18 +589,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F662D5-C154-478B-901C-CD18525D5839}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,8 +614,14 @@
       <c r="F1">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -624,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="D3" t="s">
         <v>8</v>
@@ -645,7 +656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>9</v>
@@ -669,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>10</v>
@@ -693,7 +704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>24</v>
@@ -717,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -728,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -757,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -786,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -827,18 +838,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF6D0A-3344-44E1-B4F6-C7514DC4A2F0}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -853,8 +865,14 @@
       <c r="F1">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -868,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="D3" t="s">
         <v>8</v>
@@ -889,7 +907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>9</v>
@@ -913,7 +931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>10</v>
@@ -937,7 +955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>24</v>
@@ -961,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -972,7 +990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1001,7 +1019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Got data import working; started on PDF generation
</commit_message>
<xml_diff>
--- a/test/testData.xlsx
+++ b/test/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\554766\Documents\Dataverwerking\dataverwerking\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16F7A0F-3D7C-459D-8FD4-E94B8380B64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285E4F86-6E8D-4582-9EF9-2DB83C4F4217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -197,7 +197,15 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -590,7 +598,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,16 +766,16 @@
         <v>2</v>
       </c>
       <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -796,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added split first and last names to student datasheet, should help with overflow
</commit_message>
<xml_diff>
--- a/test/testData.xlsx
+++ b/test/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\554766\Documents\Dataverwerking\dataverwerking\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285E4F86-6E8D-4582-9EF9-2DB83C4F4217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAEC77A-7D23-4496-8F3A-79B8FC9B33B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DCD764D9-00D8-4589-8408-A83FB7ACBEF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Emma</t>
   </si>
   <si>
-    <t>de Beer</t>
-  </si>
-  <si>
     <t>G1A</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Aantal vragen:</t>
+  </si>
+  <si>
+    <t>de Beer van Klaassen</t>
   </si>
 </sst>
 </file>
@@ -197,15 +197,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -564,7 +556,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +564,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -597,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F662D5-C154-478B-901C-CD18525D5839}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +617,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1">
         <v>6</v>
@@ -757,7 +749,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -783,10 +775,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -809,13 +801,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -848,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF6D0A-3344-44E1-B4F6-C7514DC4A2F0}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -876,7 +868,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1">
         <v>6</v>
@@ -1008,7 +1000,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1034,10 +1026,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1060,13 +1052,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
       </c>
       <c r="D10">
         <v>1</v>

</xml_diff>